<commit_message>
initial commit for heroku
</commit_message>
<xml_diff>
--- a/Simulation_Summary.xlsx
+++ b/Simulation_Summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Claim</t>
   </si>
@@ -85,7 +85,7 @@
     <t>Subgroup</t>
   </si>
   <si>
-    <t>Caregivers</t>
+    <t>Current WWP Members</t>
   </si>
   <si>
     <t>Number of Respondents</t>
@@ -478,8 +478,8 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
+      <c r="C3">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -489,8 +489,8 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>79.17</v>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -533,8 +533,8 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
+      <c r="C8">
+        <v>71.59</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -566,8 +566,8 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
+      <c r="C11">
+        <v>46.69</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -599,8 +599,8 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
+      <c r="C14">
+        <v>58.71</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -645,19 +645,19 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>1.4</v>
+        <v>1.339</v>
       </c>
       <c r="C18">
-        <v>79.17</v>
+        <v>76.33</v>
       </c>
       <c r="D18">
-        <v>75.95</v>
+        <v>72.06</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
       </c>
       <c r="F18">
-        <v>355</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
database update. react router working
</commit_message>
<xml_diff>
--- a/Simulation_Summary.xlsx
+++ b/Simulation_Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:E21"/>
+  <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,15 +446,23 @@
           <t>Wounded Warrior Project provides life-changing mental health treatment at no cost to warriors</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="n">
+        <v>0.7632575757575758</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0.7632575757575758</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Already Offered</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>0.7869318181818182</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Already Offered</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Already Offered</t>
         </is>
@@ -466,16 +474,22 @@
           <t>76% of warriors who complete the Wounded Warrior Project Warrior Care Network program experience fewer PTSD symptoms</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>0.7159090909090909</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Already Offered</t>
+        </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.6600378787878788</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Already Offered</t>
-        </is>
+        <v>0.6789772727272727</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0.625</v>
       </c>
     </row>
     <row r="4">
@@ -487,13 +501,17 @@
       <c r="C4" s="2" t="n">
         <v>0.7916666666666666</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Considered</t>
-        </is>
+      <c r="D4" s="2" t="n">
+        <v>0.7916666666666666</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.7253787878787878</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.7253787878787878</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0.7253787878787878</v>
       </c>
     </row>
     <row r="5">
@@ -509,10 +527,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Considered</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Considered</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Considered</t>
         </is>
@@ -529,13 +557,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Already Offered</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Considered</t>
-        </is>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.7698863636363636</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.7698863636363636</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0.7698863636363636</v>
       </c>
     </row>
     <row r="7">
@@ -545,13 +577,19 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.7632575757575758</v>
+        <v>0.728219696969697</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.7121212121212122</v>
+        <v>0.728219696969697</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.7632575757575758</v>
+        <v>0.6808712121212122</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.6808712121212122</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0.6808712121212122</v>
       </c>
     </row>
     <row r="8">
@@ -560,18 +598,22 @@
           <t>Wounded Warrior Project’s members often find a lifelong support system and the treatment and tools needed to manage their anger, heal their family and themselves</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="2" t="n">
+        <v>0.6789772727272727</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>Already Offered</t>
         </is>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>0.7575757575757576</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Already Offered</t>
-        </is>
+      <c r="E8" s="2" t="n">
+        <v>0.5492424242424242</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.5492424242424242</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0.5492424242424242</v>
       </c>
     </row>
     <row r="9">
@@ -583,13 +625,17 @@
       <c r="C9" s="2" t="n">
         <v>0.8115530303030303</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Considered</t>
-        </is>
+      <c r="D9" s="2" t="n">
+        <v>0.8115530303030303</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.8115530303030303</v>
+        <v>0.75</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0.75</v>
       </c>
     </row>
     <row r="10">
@@ -603,14 +649,22 @@
           <t>Considered</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Considered</t>
-        </is>
+      <c r="D10" s="2" t="n">
+        <v>0.8390151515151515</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Considered</t>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Excluded</t>
         </is>
       </c>
     </row>
@@ -620,20 +674,20 @@
           <t>Wounded Warrior Project offers a no-cost program for veterans designed to help warriors living with post-traumatic stress disorder (PTSD), military sexual trauma (MST) and traumatic brain injury (TBI) and their families</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Already Offered</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Already Offered</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Already Offered</t>
-        </is>
+      <c r="C11" s="2" t="n">
+        <v>0.4914772727272727</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0.4886363636363636</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.4668560606060606</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.4668560606060606</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0.4668560606060606</v>
       </c>
     </row>
     <row r="12">
@@ -647,12 +701,20 @@
           <t>Considered</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="2" t="n">
+        <v>0.8446969696969697</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>Considered</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Considered</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Considered</t>
         </is>
@@ -664,19 +726,25 @@
           <t>Wounded Warrior Project helps warriors find the treatment, tools, and resources to cope with the anger, pain, and anxiety caused by PTSD to help them feel like themselves again</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Considered</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Considered</t>
-        </is>
+      <c r="C13" s="2" t="n">
+        <v>0.84375</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.8276515151515151</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Considered</t>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Excluded</t>
         </is>
       </c>
     </row>
@@ -686,19 +754,25 @@
           <t>Warriors never pay a penny for Wounded Warrior Project’s programs and services — because they paid their dues on the battlefield</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Already Offered</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Already Offered</t>
-        </is>
+      <c r="C14" s="2" t="n">
+        <v>0.6212121212121212</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.6060606060606061</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Already Offered</t>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Excluded</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Excluded</t>
         </is>
       </c>
     </row>
@@ -717,7 +791,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Current WWP Members</t>
+          <t>Vets</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -727,7 +801,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Caregivers</t>
+          <t>Vets</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Vets</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Vets</t>
         </is>
       </c>
     </row>
@@ -738,13 +822,19 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>177</v>
+        <v>701</v>
       </c>
       <c r="D18" t="n">
         <v>701</v>
       </c>
       <c r="E18" t="n">
-        <v>355</v>
+        <v>701</v>
+      </c>
+      <c r="F18" t="n">
+        <v>701</v>
+      </c>
+      <c r="G18" t="n">
+        <v>701</v>
       </c>
     </row>
     <row r="19">
@@ -754,13 +844,19 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1.56</v>
+        <v>1.85</v>
       </c>
       <c r="D19" t="n">
-        <v>1.41</v>
+        <v>1.96</v>
       </c>
       <c r="E19" t="n">
-        <v>1.49</v>
+        <v>1.29</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.29</v>
       </c>
     </row>
     <row r="20">
@@ -770,13 +866,19 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.8285984848484849</v>
+        <v>0.84375</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0.7869318181818182</v>
+        <v>0.8446969696969697</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.8115530303030303</v>
+        <v>0.7698863636363636</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0.7698863636363636</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0.7698863636363636</v>
       </c>
     </row>
     <row r="21">
@@ -786,13 +888,19 @@
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.8409090909090908</v>
+        <v>0.9024621212121211</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0.7594696969696969</v>
+        <v>0.9223484848484848</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.8020833333333334</v>
+        <v>0.6931818181818181</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0.6931818181818181</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>0.6931818181818181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>